<commit_message>
Revert "Update to version 3.2.1"
This reverts commit b64df9b476d8d2165a8e657e3f91588ded895414.
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US_EPS\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59485A2-ADF5-4469-ABB4-3A063C7F174B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B894A-F356-4233-B257-22D3D9ACBC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1620" windowWidth="12720" windowHeight="14955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5310" yWindow="1590" windowWidth="21660" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -93,169 +93,166 @@
     <t>Dec.</t>
   </si>
   <si>
+    <t>1968.............................................................................     .</t>
+  </si>
+  <si>
     <t>–</t>
   </si>
   <si>
+    <t>1969.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1970.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1971.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1972.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1973.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1974.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1975.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1976.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1977.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1978.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1979.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1980.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1981.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1982.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1983.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1984.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1985.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1986.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1987.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1988.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1989.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1990.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1991.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1992.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1993.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1994.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1995.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1996.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1997.............................................................................      .</t>
+  </si>
+  <si>
+    <t>1998.............................................................................     .</t>
+  </si>
+  <si>
+    <t>1999.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2000.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2001.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2002.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2003.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2004.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2005.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2006.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2007.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2008.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2009.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2010.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2011.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2012.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2013.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2014.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2015.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2016.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2017.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2018.............................................................................     .</t>
+  </si>
+  <si>
+    <t>2019.............................................................................     .</t>
+  </si>
+  <si>
     <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201912.pdf</t>
-  </si>
-  <si>
-    <t>1968............................................................................. .</t>
-  </si>
-  <si>
-    <t>1969............................................................................. .</t>
-  </si>
-  <si>
-    <t>1970............................................................................. .</t>
-  </si>
-  <si>
-    <t>1971............................................................................. .</t>
-  </si>
-  <si>
-    <t>1972............................................................................. .</t>
-  </si>
-  <si>
-    <t>1973............................................................................. .</t>
-  </si>
-  <si>
-    <t>1974............................................................................. .</t>
-  </si>
-  <si>
-    <t>1975............................................................................. .</t>
-  </si>
-  <si>
-    <t>1976............................................................................. .</t>
-  </si>
-  <si>
-    <t>1977............................................................................. .</t>
-  </si>
-  <si>
-    <t>1978............................................................................. .</t>
-  </si>
-  <si>
-    <t>1979............................................................................. .</t>
-  </si>
-  <si>
-    <t>1980............................................................................. .</t>
-  </si>
-  <si>
-    <t>1981............................................................................. .</t>
-  </si>
-  <si>
-    <t>1982............................................................................. .</t>
-  </si>
-  <si>
-    <t>1983............................................................................. .</t>
-  </si>
-  <si>
-    <t>1984............................................................................. .</t>
-  </si>
-  <si>
-    <t>1985............................................................................. .</t>
-  </si>
-  <si>
-    <t>1986............................................................................. .</t>
-  </si>
-  <si>
-    <t>1987............................................................................. .</t>
-  </si>
-  <si>
-    <t>1988............................................................................. .</t>
-  </si>
-  <si>
-    <t>1989............................................................................. .</t>
-  </si>
-  <si>
-    <t>1990............................................................................. .</t>
-  </si>
-  <si>
-    <t>1991............................................................................. .</t>
-  </si>
-  <si>
-    <t>1992............................................................................. .</t>
-  </si>
-  <si>
-    <t>1993............................................................................. .</t>
-  </si>
-  <si>
-    <t>1994............................................................................. .</t>
-  </si>
-  <si>
-    <t>1995............................................................................. .</t>
-  </si>
-  <si>
-    <t>1996............................................................................. .</t>
-  </si>
-  <si>
-    <t>1997............................................................................. .</t>
-  </si>
-  <si>
-    <t>1998............................................................................. .</t>
-  </si>
-  <si>
-    <t>1999............................................................................. .</t>
-  </si>
-  <si>
-    <t>2000............................................................................. .</t>
-  </si>
-  <si>
-    <t>2001............................................................................. .</t>
-  </si>
-  <si>
-    <t>2002............................................................................. .</t>
-  </si>
-  <si>
-    <t>2003............................................................................. .</t>
-  </si>
-  <si>
-    <t>2004............................................................................. .</t>
-  </si>
-  <si>
-    <t>2005............................................................................. .</t>
-  </si>
-  <si>
-    <t>2006............................................................................. .</t>
-  </si>
-  <si>
-    <t>2007............................................................................. .</t>
-  </si>
-  <si>
-    <t>2008............................................................................. .</t>
-  </si>
-  <si>
-    <t>2009............................................................................. .</t>
-  </si>
-  <si>
-    <t>2010............................................................................. .</t>
-  </si>
-  <si>
-    <t>2011............................................................................. .</t>
-  </si>
-  <si>
-    <t>2012............................................................................. .</t>
-  </si>
-  <si>
-    <t>2013............................................................................. .</t>
-  </si>
-  <si>
-    <t>2014............................................................................. .</t>
-  </si>
-  <si>
-    <t>2015............................................................................. .</t>
-  </si>
-  <si>
-    <t>2016............................................................................. .</t>
-  </si>
-  <si>
-    <t>2017............................................................................. .</t>
-  </si>
-  <si>
-    <t>2018............................................................................. .</t>
-  </si>
-  <si>
-    <t>2019............................................................................. .</t>
-  </si>
-  <si>
-    <t>2020............................................................................. .</t>
   </si>
 </sst>
 </file>
@@ -667,9 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -698,7 +693,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,11 +732,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -797,13 +790,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>34.799999999999997</v>
@@ -817,13 +810,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>36.700000000000003</v>
@@ -837,13 +830,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>38.799999999999997</v>
@@ -857,13 +850,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>40.5</v>
@@ -877,13 +870,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>41.8</v>
@@ -897,13 +890,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>44.4</v>
@@ -917,13 +910,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>49.3</v>
@@ -937,13 +930,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>53.8</v>
@@ -957,13 +950,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14">
         <v>56.9</v>
@@ -977,13 +970,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15">
         <v>60.6</v>
@@ -997,13 +990,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16">
         <v>65.2</v>
@@ -1017,13 +1010,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>72.599999999999994</v>
@@ -1037,13 +1030,13 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18">
         <v>82.4</v>
@@ -1057,13 +1050,13 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19">
         <v>90.9</v>
@@ -1077,13 +1070,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20">
         <v>96.5</v>
@@ -1097,13 +1090,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21">
         <v>99.6</v>
@@ -1117,7 +1110,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>102.9</v>
@@ -1137,7 +1130,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>106.6</v>
@@ -1157,7 +1150,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24">
         <v>109.1</v>
@@ -1177,7 +1170,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25">
         <v>112.4</v>
@@ -1197,7 +1190,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26">
         <v>116.8</v>
@@ -1217,7 +1210,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>122.7</v>
@@ -1237,7 +1230,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28">
         <v>128.69999999999999</v>
@@ -1261,7 +1254,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>135.19999999999999</v>
@@ -1288,7 +1281,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>139.19999999999999</v>
@@ -1315,7 +1308,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31">
         <v>143.69999999999999</v>
@@ -1342,7 +1335,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32">
         <v>147.19999999999999</v>
@@ -1369,7 +1362,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33">
         <v>151.5</v>
@@ -1396,7 +1389,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34">
         <v>155.80000000000001</v>
@@ -1423,7 +1416,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35">
         <v>159.9</v>
@@ -1450,7 +1443,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36">
         <v>162.30000000000001</v>
@@ -1477,7 +1470,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37">
         <v>165.4</v>
@@ -1504,7 +1497,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38">
         <v>170.8</v>
@@ -1531,7 +1524,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39">
         <v>176.6</v>
@@ -1558,7 +1551,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40">
         <v>178.9</v>
@@ -1585,7 +1578,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41">
         <v>183.3</v>
@@ -1612,7 +1605,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B42">
         <v>187.6</v>
@@ -1639,7 +1632,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43">
         <v>193.2</v>
@@ -1666,7 +1659,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44">
         <v>200.6</v>
@@ -1693,7 +1686,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45">
         <v>205.709</v>
@@ -1720,7 +1713,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46">
         <v>214.429</v>
@@ -1747,7 +1740,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47">
         <v>213.13900000000001</v>
@@ -1774,7 +1767,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48">
         <v>217.535</v>
@@ -1801,7 +1794,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49">
         <v>223.59800000000001</v>
@@ -1828,7 +1821,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50">
         <v>228.85</v>
@@ -1855,7 +1848,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51">
         <v>232.36600000000001</v>
@@ -1882,7 +1875,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52">
         <v>236.38399999999999</v>
@@ -1909,7 +1902,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53">
         <v>236.26499999999999</v>
@@ -1936,7 +1929,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54">
         <v>238.77799999999999</v>
@@ -1963,7 +1956,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55">
         <v>244.07599999999999</v>
@@ -1990,7 +1983,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56">
         <v>250.089</v>
@@ -2017,7 +2010,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57">
         <v>254.41200000000001</v>
@@ -2035,32 +2028,8 @@
         <v>1.8</v>
       </c>
       <c r="G57" s="6">
-        <f>$D$50/D57</f>
+        <f t="shared" si="0"/>
         <v>0.89805481563188172</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58">
-        <v>257.55700000000002</v>
-      </c>
-      <c r="C58">
-        <v>260.065</v>
-      </c>
-      <c r="D58">
-        <v>258.81099999999998</v>
-      </c>
-      <c r="E58">
-        <v>1.4</v>
-      </c>
-      <c r="F58">
-        <v>1.2</v>
-      </c>
-      <c r="G58" s="6">
-        <f>$D$50/D58</f>
-        <v>0.88711067149387013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to version 3.2.1
</commit_message>
<xml_diff>
--- a/InputData/cpi.xlsx
+++ b/InputData/cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\US_EPS\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B894A-F356-4233-B257-22D3D9ACBC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59485A2-ADF5-4469-ABB4-3A063C7F174B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="1590" windowWidth="21660" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1620" windowWidth="12720" windowHeight="14955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
   <si>
     <t>CPI Consumer Price Index</t>
   </si>
@@ -93,166 +93,169 @@
     <t>Dec.</t>
   </si>
   <si>
-    <t>1968.............................................................................     .</t>
-  </si>
-  <si>
     <t>–</t>
   </si>
   <si>
-    <t>1969.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1970.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1971.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1972.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1973.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1974.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1975.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1976.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1977.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1978.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1979.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1980.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1981.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1982.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1983.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1984.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1985.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1986.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1987.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1988.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1989.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1990.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1991.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1992.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1993.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1994.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1995.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1996.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1997.............................................................................      .</t>
-  </si>
-  <si>
-    <t>1998.............................................................................     .</t>
-  </si>
-  <si>
-    <t>1999.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2000.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2001.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2002.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2003.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2004.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2005.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2006.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2007.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2008.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2009.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2010.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2011.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2012.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2013.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2014.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2015.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2016.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2017.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2018.............................................................................     .</t>
-  </si>
-  <si>
-    <t>2019.............................................................................     .</t>
-  </si>
-  <si>
     <t>https://www.bls.gov/cpi/tables/supplemental-files/historical-cpi-u-201912.pdf</t>
+  </si>
+  <si>
+    <t>1968............................................................................. .</t>
+  </si>
+  <si>
+    <t>1969............................................................................. .</t>
+  </si>
+  <si>
+    <t>1970............................................................................. .</t>
+  </si>
+  <si>
+    <t>1971............................................................................. .</t>
+  </si>
+  <si>
+    <t>1972............................................................................. .</t>
+  </si>
+  <si>
+    <t>1973............................................................................. .</t>
+  </si>
+  <si>
+    <t>1974............................................................................. .</t>
+  </si>
+  <si>
+    <t>1975............................................................................. .</t>
+  </si>
+  <si>
+    <t>1976............................................................................. .</t>
+  </si>
+  <si>
+    <t>1977............................................................................. .</t>
+  </si>
+  <si>
+    <t>1978............................................................................. .</t>
+  </si>
+  <si>
+    <t>1979............................................................................. .</t>
+  </si>
+  <si>
+    <t>1980............................................................................. .</t>
+  </si>
+  <si>
+    <t>1981............................................................................. .</t>
+  </si>
+  <si>
+    <t>1982............................................................................. .</t>
+  </si>
+  <si>
+    <t>1983............................................................................. .</t>
+  </si>
+  <si>
+    <t>1984............................................................................. .</t>
+  </si>
+  <si>
+    <t>1985............................................................................. .</t>
+  </si>
+  <si>
+    <t>1986............................................................................. .</t>
+  </si>
+  <si>
+    <t>1987............................................................................. .</t>
+  </si>
+  <si>
+    <t>1988............................................................................. .</t>
+  </si>
+  <si>
+    <t>1989............................................................................. .</t>
+  </si>
+  <si>
+    <t>1990............................................................................. .</t>
+  </si>
+  <si>
+    <t>1991............................................................................. .</t>
+  </si>
+  <si>
+    <t>1992............................................................................. .</t>
+  </si>
+  <si>
+    <t>1993............................................................................. .</t>
+  </si>
+  <si>
+    <t>1994............................................................................. .</t>
+  </si>
+  <si>
+    <t>1995............................................................................. .</t>
+  </si>
+  <si>
+    <t>1996............................................................................. .</t>
+  </si>
+  <si>
+    <t>1997............................................................................. .</t>
+  </si>
+  <si>
+    <t>1998............................................................................. .</t>
+  </si>
+  <si>
+    <t>1999............................................................................. .</t>
+  </si>
+  <si>
+    <t>2000............................................................................. .</t>
+  </si>
+  <si>
+    <t>2001............................................................................. .</t>
+  </si>
+  <si>
+    <t>2002............................................................................. .</t>
+  </si>
+  <si>
+    <t>2003............................................................................. .</t>
+  </si>
+  <si>
+    <t>2004............................................................................. .</t>
+  </si>
+  <si>
+    <t>2005............................................................................. .</t>
+  </si>
+  <si>
+    <t>2006............................................................................. .</t>
+  </si>
+  <si>
+    <t>2007............................................................................. .</t>
+  </si>
+  <si>
+    <t>2008............................................................................. .</t>
+  </si>
+  <si>
+    <t>2009............................................................................. .</t>
+  </si>
+  <si>
+    <t>2010............................................................................. .</t>
+  </si>
+  <si>
+    <t>2011............................................................................. .</t>
+  </si>
+  <si>
+    <t>2012............................................................................. .</t>
+  </si>
+  <si>
+    <t>2013............................................................................. .</t>
+  </si>
+  <si>
+    <t>2014............................................................................. .</t>
+  </si>
+  <si>
+    <t>2015............................................................................. .</t>
+  </si>
+  <si>
+    <t>2016............................................................................. .</t>
+  </si>
+  <si>
+    <t>2017............................................................................. .</t>
+  </si>
+  <si>
+    <t>2018............................................................................. .</t>
+  </si>
+  <si>
+    <t>2019............................................................................. .</t>
+  </si>
+  <si>
+    <t>2020............................................................................. .</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -693,7 +698,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,9 +737,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -790,13 +797,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>34.799999999999997</v>
@@ -810,13 +817,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>36.700000000000003</v>
@@ -830,13 +837,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>38.799999999999997</v>
@@ -850,13 +857,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>40.5</v>
@@ -870,13 +877,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>41.8</v>
@@ -890,13 +897,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>44.4</v>
@@ -910,13 +917,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>49.3</v>
@@ -930,13 +937,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>53.8</v>
@@ -950,13 +957,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>56.9</v>
@@ -970,13 +977,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>60.6</v>
@@ -990,13 +997,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>65.2</v>
@@ -1010,13 +1017,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>72.599999999999994</v>
@@ -1030,13 +1037,13 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18">
         <v>82.4</v>
@@ -1050,13 +1057,13 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19">
         <v>90.9</v>
@@ -1070,13 +1077,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20">
         <v>96.5</v>
@@ -1090,13 +1097,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21">
         <v>99.6</v>
@@ -1110,7 +1117,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>102.9</v>
@@ -1130,7 +1137,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>106.6</v>
@@ -1150,7 +1157,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>109.1</v>
@@ -1170,7 +1177,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25">
         <v>112.4</v>
@@ -1190,7 +1197,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>116.8</v>
@@ -1210,7 +1217,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>122.7</v>
@@ -1230,7 +1237,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>128.69999999999999</v>
@@ -1254,7 +1261,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29">
         <v>135.19999999999999</v>
@@ -1281,7 +1288,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B30">
         <v>139.19999999999999</v>
@@ -1308,7 +1315,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31">
         <v>143.69999999999999</v>
@@ -1335,7 +1342,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>147.19999999999999</v>
@@ -1362,7 +1369,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>151.5</v>
@@ -1389,7 +1396,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34">
         <v>155.80000000000001</v>
@@ -1416,7 +1423,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35">
         <v>159.9</v>
@@ -1443,7 +1450,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B36">
         <v>162.30000000000001</v>
@@ -1470,7 +1477,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B37">
         <v>165.4</v>
@@ -1497,7 +1504,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B38">
         <v>170.8</v>
@@ -1524,7 +1531,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B39">
         <v>176.6</v>
@@ -1551,7 +1558,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B40">
         <v>178.9</v>
@@ -1578,7 +1585,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B41">
         <v>183.3</v>
@@ -1605,7 +1612,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B42">
         <v>187.6</v>
@@ -1632,7 +1639,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B43">
         <v>193.2</v>
@@ -1659,7 +1666,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44">
         <v>200.6</v>
@@ -1686,7 +1693,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45">
         <v>205.709</v>
@@ -1713,7 +1720,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46">
         <v>214.429</v>
@@ -1740,7 +1747,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B47">
         <v>213.13900000000001</v>
@@ -1767,7 +1774,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B48">
         <v>217.535</v>
@@ -1794,7 +1801,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B49">
         <v>223.59800000000001</v>
@@ -1821,7 +1828,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B50">
         <v>228.85</v>
@@ -1848,7 +1855,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51">
         <v>232.36600000000001</v>
@@ -1875,7 +1882,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B52">
         <v>236.38399999999999</v>
@@ -1902,7 +1909,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B53">
         <v>236.26499999999999</v>
@@ -1929,7 +1936,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B54">
         <v>238.77799999999999</v>
@@ -1956,7 +1963,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B55">
         <v>244.07599999999999</v>
@@ -1983,7 +1990,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B56">
         <v>250.089</v>
@@ -2010,7 +2017,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B57">
         <v>254.41200000000001</v>
@@ -2028,8 +2035,32 @@
         <v>1.8</v>
       </c>
       <c r="G57" s="6">
-        <f t="shared" si="0"/>
+        <f>$D$50/D57</f>
         <v>0.89805481563188172</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58">
+        <v>257.55700000000002</v>
+      </c>
+      <c r="C58">
+        <v>260.065</v>
+      </c>
+      <c r="D58">
+        <v>258.81099999999998</v>
+      </c>
+      <c r="E58">
+        <v>1.4</v>
+      </c>
+      <c r="F58">
+        <v>1.2</v>
+      </c>
+      <c r="G58" s="6">
+        <f>$D$50/D58</f>
+        <v>0.88711067149387013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>